<commit_message>
Update Pertanggal 22 November 2023 17:43 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Accounting.TblChartOfAccount.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Accounting.TblChartOfAccount.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="5850" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9360" windowHeight="3330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Auto Link" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="QDC COA" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="853">
   <si>
     <t>RAW COA STRUCTURE</t>
   </si>
@@ -2144,6 +2145,444 @@
   </si>
   <si>
     <t>Dll…</t>
+  </si>
+  <si>
+    <t>Aset</t>
+  </si>
+  <si>
+    <t>Hutang</t>
+  </si>
+  <si>
+    <t>Modal</t>
+  </si>
+  <si>
+    <t>Pendapatan</t>
+  </si>
+  <si>
+    <t>HPP (COGS)</t>
+  </si>
+  <si>
+    <t>Biaya Adm &amp; Umum</t>
+  </si>
+  <si>
+    <t>Pendapatan Lain2</t>
+  </si>
+  <si>
+    <t>8-00.000.000</t>
+  </si>
+  <si>
+    <t>Biaya Lain2</t>
+  </si>
+  <si>
+    <t>Other Current Asset</t>
+  </si>
+  <si>
+    <t>7-0000</t>
+  </si>
+  <si>
+    <t>Aset Tetap</t>
+  </si>
+  <si>
+    <t>Aset Lancar</t>
+  </si>
+  <si>
+    <t>1-1102.01</t>
+  </si>
+  <si>
+    <t>1-1102.02</t>
+  </si>
+  <si>
+    <t>BCA IDR 001</t>
+  </si>
+  <si>
+    <t>1-1102.01.01</t>
+  </si>
+  <si>
+    <t>1-1102.01.02</t>
+  </si>
+  <si>
+    <t>BCA IDR 021</t>
+  </si>
+  <si>
+    <t>1-1102.02.01</t>
+  </si>
+  <si>
+    <t>BRI IDR 341</t>
+  </si>
+  <si>
+    <t>1-1102.01.03</t>
+  </si>
+  <si>
+    <t>MT IDR</t>
+  </si>
+  <si>
+    <t>1-1102.01.99</t>
+  </si>
+  <si>
+    <t>MT USD</t>
+  </si>
+  <si>
+    <t>1-1102.02.99</t>
+  </si>
+  <si>
+    <t>BNI USD 322</t>
+  </si>
+  <si>
+    <t>1-1101.01</t>
+  </si>
+  <si>
+    <t>PettyCash IDR</t>
+  </si>
+  <si>
+    <t>1-1101.01.01</t>
+  </si>
+  <si>
+    <t>Petty Cash IDR Kantor Pusat</t>
+  </si>
+  <si>
+    <t>1-1101.01.02</t>
+  </si>
+  <si>
+    <t>Petty Cash IDR Project ABC</t>
+  </si>
+  <si>
+    <t>1-1101.01.03</t>
+  </si>
+  <si>
+    <t>Petty Cash IDR Project XYZ</t>
+  </si>
+  <si>
+    <t>LEVEL 3</t>
+  </si>
+  <si>
+    <t>LEVEL 4</t>
+  </si>
+  <si>
+    <t>LEVEL 5</t>
+  </si>
+  <si>
+    <t>LEVEL 6</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Piutang Usaha</t>
+  </si>
+  <si>
+    <t>1-1201.01</t>
+  </si>
+  <si>
+    <t>1-1201.02</t>
+  </si>
+  <si>
+    <t>1-1202</t>
+  </si>
+  <si>
+    <t>Cadangan Kerugian Piutang</t>
+  </si>
+  <si>
+    <t>1-1202.01</t>
+  </si>
+  <si>
+    <t>1-1202.02</t>
+  </si>
+  <si>
+    <t>Cadangan Kerugian Piutang IDR</t>
+  </si>
+  <si>
+    <t>Cadangan Kerugian Piutang USD</t>
+  </si>
+  <si>
+    <t>Piutang Non Usaha</t>
+  </si>
+  <si>
+    <t>1-1203.01</t>
+  </si>
+  <si>
+    <t>Piutang Non Usaha IDR</t>
+  </si>
+  <si>
+    <t>1-1204</t>
+  </si>
+  <si>
+    <t>Piutang Antar Perusahaan</t>
+  </si>
+  <si>
+    <t>1-1204.01</t>
+  </si>
+  <si>
+    <t>Piutang Antar Perusahaan - IDR</t>
+  </si>
+  <si>
+    <t>1-1204.01.01</t>
+  </si>
+  <si>
+    <t>Piutang Antar Perusahaan - IDR - IMD</t>
+  </si>
+  <si>
+    <t>Piutang Antar Perusahaan - IDR - EML</t>
+  </si>
+  <si>
+    <t>1-1204.01.02</t>
+  </si>
+  <si>
+    <t>Inventory - IDR</t>
+  </si>
+  <si>
+    <t>1-1301</t>
+  </si>
+  <si>
+    <t>1-1301.01</t>
+  </si>
+  <si>
+    <t>1-1301.01.01</t>
+  </si>
+  <si>
+    <t>Inventory IDR Kantor Pusat</t>
+  </si>
+  <si>
+    <t>Inventory IDR Project ABC</t>
+  </si>
+  <si>
+    <t>1-1301.01.02</t>
+  </si>
+  <si>
+    <t>1-9900</t>
+  </si>
+  <si>
+    <t>Biaya Dibayar Dimuka</t>
+  </si>
+  <si>
+    <t>Pajak Dibayar Dimuka</t>
+  </si>
+  <si>
+    <t>Perlengkapan Kantor</t>
+  </si>
+  <si>
+    <t>Uang Muka</t>
+  </si>
+  <si>
+    <t>1-9901</t>
+  </si>
+  <si>
+    <t>1-9902</t>
+  </si>
+  <si>
+    <t>1-9903</t>
+  </si>
+  <si>
+    <t>1-9904</t>
+  </si>
+  <si>
+    <t>1-9905</t>
+  </si>
+  <si>
+    <t>1-9999</t>
+  </si>
+  <si>
+    <t>1-9901.01</t>
+  </si>
+  <si>
+    <t>1-9902.01</t>
+  </si>
+  <si>
+    <t>1-9903.01</t>
+  </si>
+  <si>
+    <t>1-9999.01</t>
+  </si>
+  <si>
+    <t>Paid in Advance - IDR</t>
+  </si>
+  <si>
+    <t>Suspense - IDR</t>
+  </si>
+  <si>
+    <t>Security Deposit - IDR</t>
+  </si>
+  <si>
+    <t>Other Prepayment - IDR</t>
+  </si>
+  <si>
+    <t>VAT IN</t>
+  </si>
+  <si>
+    <t>1-1501</t>
+  </si>
+  <si>
+    <t>1-1502</t>
+  </si>
+  <si>
+    <t>1-1503</t>
+  </si>
+  <si>
+    <t>1-9904.01</t>
+  </si>
+  <si>
+    <t>1-9905.01</t>
+  </si>
+  <si>
+    <t>Unbilled Receivable - IDR</t>
+  </si>
+  <si>
+    <t>Work in Progress - IDR</t>
+  </si>
+  <si>
+    <t>1-1504</t>
+  </si>
+  <si>
+    <t>1-1501.01</t>
+  </si>
+  <si>
+    <t>1-1502.01</t>
+  </si>
+  <si>
+    <t>1-1503.01</t>
+  </si>
+  <si>
+    <t>1-1504.01</t>
+  </si>
+  <si>
+    <t>VAT IN - IDR</t>
+  </si>
+  <si>
+    <t>Prepaid Tax 22 - IDR</t>
+  </si>
+  <si>
+    <t>Prepaid Tax 23 - IDR</t>
+  </si>
+  <si>
+    <t>Prepaid Tax 25 - IDR</t>
+  </si>
+  <si>
+    <t>Investasi Jangka Panjang</t>
+  </si>
+  <si>
+    <t>Investasi Saham</t>
+  </si>
+  <si>
+    <t>1-2101</t>
+  </si>
+  <si>
+    <t>Investasi Saham IMD</t>
+  </si>
+  <si>
+    <t>Investasi Saham EML</t>
+  </si>
+  <si>
+    <t>1-2101.01</t>
+  </si>
+  <si>
+    <t>1-2102</t>
+  </si>
+  <si>
+    <t>1-2103</t>
+  </si>
+  <si>
+    <t>1-2102.01</t>
+  </si>
+  <si>
+    <t>1-2103.01</t>
+  </si>
+  <si>
+    <t>Investasi Saham IMD - IDR</t>
+  </si>
+  <si>
+    <t>Investasi Saham EML - IDR</t>
+  </si>
+  <si>
+    <t>Investasi Saham DHD - IDR</t>
+  </si>
+  <si>
+    <t>Aktiva Tetap</t>
+  </si>
+  <si>
+    <t>1-3200</t>
+  </si>
+  <si>
+    <t>1-3101</t>
+  </si>
+  <si>
+    <t>1-3102</t>
+  </si>
+  <si>
+    <t>1-3103</t>
+  </si>
+  <si>
+    <t>1-3104</t>
+  </si>
+  <si>
+    <t>1-3105</t>
+  </si>
+  <si>
+    <t>1-3106</t>
+  </si>
+  <si>
+    <t>1-3107</t>
+  </si>
+  <si>
+    <t>1-3108</t>
+  </si>
+  <si>
+    <t>1-3109</t>
+  </si>
+  <si>
+    <t>1-3110</t>
+  </si>
+  <si>
+    <t>Acc Penyusutan</t>
+  </si>
+  <si>
+    <t>1-3201</t>
+  </si>
+  <si>
+    <t>1-3202</t>
+  </si>
+  <si>
+    <t>1-3203</t>
+  </si>
+  <si>
+    <t>1-3204</t>
+  </si>
+  <si>
+    <t>1-3205</t>
+  </si>
+  <si>
+    <t>1-3206</t>
+  </si>
+  <si>
+    <t>1-3207</t>
+  </si>
+  <si>
+    <t>1-3208</t>
+  </si>
+  <si>
+    <t>1-3209</t>
+  </si>
+  <si>
+    <t>1-3210</t>
+  </si>
+  <si>
+    <t>1-3111</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Aktiva Lain2</t>
+  </si>
+  <si>
+    <t>Aktiva Tetap Tidak Berwujud</t>
+  </si>
+  <si>
+    <t>Pre Ops Project</t>
+  </si>
+  <si>
+    <t>1-5100</t>
+  </si>
+  <si>
+    <t>1-5103</t>
   </si>
 </sst>
 </file>
@@ -2214,7 +2653,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2237,12 +2676,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -2273,6 +2736,27 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2784,11 +3268,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AO344"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="18" ySplit="4" topLeftCell="S90" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="18" ySplit="4" topLeftCell="S109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J100" sqref="J100"/>
+      <selection pane="bottomRight" activeCell="Q115" sqref="Q115:Q117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37459,4 +37943,1817 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M95"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I60" sqref="I60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="17" customWidth="1"/>
+    <col min="10" max="10" width="8" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="17" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18" t="s">
+        <v>742</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
+        <v>743</v>
+      </c>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
+        <v>744</v>
+      </c>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18" t="s">
+        <v>745</v>
+      </c>
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="J3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>707</v>
+      </c>
+      <c r="D4" s="20"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="21"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>719</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+    </row>
+    <row r="6" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22" t="s">
+        <v>734</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>735</v>
+      </c>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22" t="s">
+        <v>736</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22" t="s">
+        <v>738</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22" t="s">
+        <v>740</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>676</v>
+      </c>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22" t="s">
+        <v>720</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>682</v>
+      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22" t="s">
+        <v>723</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22" t="s">
+        <v>724</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22" t="s">
+        <v>728</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22" t="s">
+        <v>730</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22" t="s">
+        <v>721</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>683</v>
+      </c>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22" t="s">
+        <v>726</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22" t="s">
+        <v>732</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>747</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>748</v>
+      </c>
+      <c r="K22" s="22" t="s">
+        <v>696</v>
+      </c>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22" t="s">
+        <v>749</v>
+      </c>
+      <c r="K23" s="22" t="s">
+        <v>697</v>
+      </c>
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+    </row>
+    <row r="24" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22" t="s">
+        <v>750</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>752</v>
+      </c>
+      <c r="K24" s="22" t="s">
+        <v>754</v>
+      </c>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+    </row>
+    <row r="25" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22" t="s">
+        <v>753</v>
+      </c>
+      <c r="K25" s="22" t="s">
+        <v>755</v>
+      </c>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+    </row>
+    <row r="26" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>756</v>
+      </c>
+      <c r="J26" s="22" t="s">
+        <v>757</v>
+      </c>
+      <c r="K26" s="22" t="s">
+        <v>758</v>
+      </c>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+    </row>
+    <row r="27" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22" t="s">
+        <v>759</v>
+      </c>
+      <c r="I27" s="22" t="s">
+        <v>760</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>761</v>
+      </c>
+      <c r="K27" s="22" t="s">
+        <v>762</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>763</v>
+      </c>
+      <c r="M27" s="22" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22" t="s">
+        <v>766</v>
+      </c>
+      <c r="M28" s="22" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>768</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>769</v>
+      </c>
+      <c r="K29" s="22" t="s">
+        <v>767</v>
+      </c>
+      <c r="L29" s="22" t="s">
+        <v>770</v>
+      </c>
+      <c r="M29" s="22" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22" t="s">
+        <v>773</v>
+      </c>
+      <c r="M30" s="22" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>775</v>
+      </c>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+    </row>
+    <row r="32" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>776</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="I32" s="22" t="s">
+        <v>793</v>
+      </c>
+      <c r="J32" s="22" t="s">
+        <v>802</v>
+      </c>
+      <c r="K32" s="22" t="s">
+        <v>806</v>
+      </c>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22" t="s">
+        <v>795</v>
+      </c>
+      <c r="I33" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="J33" s="22" t="s">
+        <v>803</v>
+      </c>
+      <c r="K33" s="22" t="s">
+        <v>807</v>
+      </c>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22" t="s">
+        <v>796</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="J34" s="22" t="s">
+        <v>804</v>
+      </c>
+      <c r="K34" s="22" t="s">
+        <v>808</v>
+      </c>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>805</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>809</v>
+      </c>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+    </row>
+    <row r="36" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>777</v>
+      </c>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>778</v>
+      </c>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+    </row>
+    <row r="39" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="23" t="s">
+        <v>774</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>716</v>
+      </c>
+      <c r="H39" s="23" t="s">
+        <v>779</v>
+      </c>
+      <c r="I39" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="J39" s="23" t="s">
+        <v>785</v>
+      </c>
+      <c r="K39" s="22" t="s">
+        <v>789</v>
+      </c>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="23" t="s">
+        <v>780</v>
+      </c>
+      <c r="I40" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="J40" s="23" t="s">
+        <v>786</v>
+      </c>
+      <c r="K40" s="22" t="s">
+        <v>790</v>
+      </c>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="23" t="s">
+        <v>781</v>
+      </c>
+      <c r="I41" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>787</v>
+      </c>
+      <c r="K41" s="22" t="s">
+        <v>791</v>
+      </c>
+      <c r="L41" s="22"/>
+      <c r="M41" s="22"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="23" t="s">
+        <v>782</v>
+      </c>
+      <c r="I42" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="J42" s="23" t="s">
+        <v>797</v>
+      </c>
+      <c r="K42" s="22" t="s">
+        <v>799</v>
+      </c>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="I43" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>798</v>
+      </c>
+      <c r="K43" s="22" t="s">
+        <v>800</v>
+      </c>
+      <c r="L43" s="22"/>
+      <c r="M43" s="22"/>
+    </row>
+    <row r="44" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="23" t="s">
+        <v>784</v>
+      </c>
+      <c r="I44" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="J44" s="23" t="s">
+        <v>788</v>
+      </c>
+      <c r="K44" s="22" t="s">
+        <v>792</v>
+      </c>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+    </row>
+    <row r="45" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>810</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>811</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>812</v>
+      </c>
+      <c r="I45" s="22" t="s">
+        <v>813</v>
+      </c>
+      <c r="J45" s="23" t="s">
+        <v>815</v>
+      </c>
+      <c r="K45" s="22" t="s">
+        <v>820</v>
+      </c>
+      <c r="L45" s="22"/>
+      <c r="M45" s="22"/>
+    </row>
+    <row r="46" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="23" t="s">
+        <v>816</v>
+      </c>
+      <c r="I46" s="22" t="s">
+        <v>814</v>
+      </c>
+      <c r="J46" s="23" t="s">
+        <v>818</v>
+      </c>
+      <c r="K46" s="22" t="s">
+        <v>821</v>
+      </c>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
+    </row>
+    <row r="47" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="23"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="23" t="s">
+        <v>817</v>
+      </c>
+      <c r="I47" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="J47" s="23" t="s">
+        <v>819</v>
+      </c>
+      <c r="K47" s="22" t="s">
+        <v>822</v>
+      </c>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
+    </row>
+    <row r="48" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>823</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>718</v>
+      </c>
+      <c r="H48" s="23" t="s">
+        <v>825</v>
+      </c>
+      <c r="I48" s="17" t="s">
+        <v>847</v>
+      </c>
+      <c r="J48" s="23"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="22"/>
+    </row>
+    <row r="49" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="23" t="s">
+        <v>826</v>
+      </c>
+      <c r="I49" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="J49" s="23"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="22"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="23" t="s">
+        <v>827</v>
+      </c>
+      <c r="I50" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="J50" s="23"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="22"/>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="23" t="s">
+        <v>828</v>
+      </c>
+      <c r="I51" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="J51" s="23"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+    </row>
+    <row r="52" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="I52" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="J52" s="23"/>
+      <c r="K52" s="22"/>
+      <c r="L52" s="22"/>
+      <c r="M52" s="22"/>
+    </row>
+    <row r="53" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="23" t="s">
+        <v>830</v>
+      </c>
+      <c r="I53" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="J53" s="23"/>
+      <c r="K53" s="22"/>
+      <c r="L53" s="22"/>
+      <c r="M53" s="22"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="23" t="s">
+        <v>831</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="J54" s="23"/>
+      <c r="K54" s="22"/>
+      <c r="L54" s="22"/>
+      <c r="M54" s="22"/>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="23" t="s">
+        <v>832</v>
+      </c>
+      <c r="I55" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="J55" s="23"/>
+      <c r="K55" s="22"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="22"/>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="23" t="s">
+        <v>833</v>
+      </c>
+      <c r="I56" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="J56" s="23"/>
+      <c r="K56" s="22"/>
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="23" t="s">
+        <v>834</v>
+      </c>
+      <c r="I57" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="J57" s="23"/>
+      <c r="K57" s="22"/>
+      <c r="L57" s="22"/>
+      <c r="M57" s="22"/>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="23" t="s">
+        <v>846</v>
+      </c>
+      <c r="I58" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="J58" s="23"/>
+      <c r="K58" s="22"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="22"/>
+    </row>
+    <row r="59" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="23" t="s">
+        <v>824</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>835</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>836</v>
+      </c>
+      <c r="I59" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="J59" s="23"/>
+      <c r="K59" s="22"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="22"/>
+    </row>
+    <row r="60" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="I60" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="J60" s="23"/>
+      <c r="K60" s="22"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="22"/>
+    </row>
+    <row r="61" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="22"/>
+      <c r="H61" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="I61" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="J61" s="23"/>
+      <c r="K61" s="22"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+    </row>
+    <row r="62" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="22"/>
+      <c r="H62" s="23" t="s">
+        <v>839</v>
+      </c>
+      <c r="I62" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="J62" s="23"/>
+      <c r="K62" s="22"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+    </row>
+    <row r="63" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="23" t="s">
+        <v>840</v>
+      </c>
+      <c r="I63" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="J63" s="23"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
+    </row>
+    <row r="64" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="22"/>
+      <c r="H64" s="23" t="s">
+        <v>841</v>
+      </c>
+      <c r="I64" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="J64" s="23"/>
+      <c r="K64" s="22"/>
+      <c r="L64" s="22"/>
+      <c r="M64" s="22"/>
+    </row>
+    <row r="65" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="23" t="s">
+        <v>842</v>
+      </c>
+      <c r="I65" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="J65" s="23"/>
+      <c r="K65" s="22"/>
+      <c r="L65" s="22"/>
+      <c r="M65" s="22"/>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B66" s="22"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="23" t="s">
+        <v>843</v>
+      </c>
+      <c r="I66" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="J66" s="23"/>
+      <c r="K66" s="22"/>
+      <c r="L66" s="22"/>
+      <c r="M66" s="22"/>
+    </row>
+    <row r="67" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="22"/>
+      <c r="H67" s="23" t="s">
+        <v>844</v>
+      </c>
+      <c r="I67" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="J67" s="23"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
+    </row>
+    <row r="68" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="22"/>
+      <c r="H68" s="23" t="s">
+        <v>845</v>
+      </c>
+      <c r="I68" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="J68" s="23"/>
+      <c r="K68" s="22"/>
+      <c r="L68" s="22"/>
+      <c r="M68" s="22"/>
+    </row>
+    <row r="69" spans="2:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>849</v>
+      </c>
+      <c r="F69" s="23"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="22"/>
+      <c r="L69" s="22"/>
+      <c r="M69" s="22"/>
+    </row>
+    <row r="70" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>848</v>
+      </c>
+      <c r="F70" s="23" t="s">
+        <v>851</v>
+      </c>
+      <c r="G70" s="22" t="s">
+        <v>850</v>
+      </c>
+      <c r="H70" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="I70" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="J70" s="23"/>
+      <c r="K70" s="22"/>
+      <c r="L70" s="22"/>
+      <c r="M70" s="22"/>
+    </row>
+    <row r="71" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="I71" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="J71" s="23"/>
+      <c r="K71" s="22"/>
+      <c r="L71" s="22"/>
+      <c r="M71" s="22"/>
+    </row>
+    <row r="72" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="23" t="s">
+        <v>852</v>
+      </c>
+      <c r="I72" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J72" s="23"/>
+      <c r="K72" s="22"/>
+      <c r="L72" s="22"/>
+      <c r="M72" s="22"/>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="22"/>
+      <c r="L73" s="22"/>
+      <c r="M73" s="22"/>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B74" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>708</v>
+      </c>
+      <c r="D74" s="23"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="23"/>
+      <c r="K74" s="22"/>
+      <c r="L74" s="23"/>
+      <c r="M74" s="22"/>
+    </row>
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="H75" s="22"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
+      <c r="K75" s="22"/>
+      <c r="L75" s="22"/>
+      <c r="M75" s="22"/>
+    </row>
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B76" s="22"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="22"/>
+      <c r="H76" s="22"/>
+      <c r="I76" s="22"/>
+      <c r="J76" s="22"/>
+      <c r="K76" s="22"/>
+      <c r="L76" s="22"/>
+      <c r="M76" s="22"/>
+    </row>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B77" s="22"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
+      <c r="G77" s="22"/>
+      <c r="H77" s="22"/>
+      <c r="I77" s="22"/>
+      <c r="J77" s="22"/>
+      <c r="K77" s="22"/>
+      <c r="L77" s="22"/>
+      <c r="M77" s="22"/>
+    </row>
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B78" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>709</v>
+      </c>
+      <c r="D78" s="23"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="22"/>
+      <c r="H78" s="23"/>
+      <c r="I78" s="22"/>
+      <c r="J78" s="23"/>
+      <c r="K78" s="22"/>
+      <c r="L78" s="23"/>
+      <c r="M78" s="22"/>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="22"/>
+      <c r="I79" s="22"/>
+      <c r="J79" s="22"/>
+      <c r="K79" s="22"/>
+      <c r="L79" s="22"/>
+      <c r="M79" s="22"/>
+    </row>
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="22"/>
+      <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
+      <c r="J80" s="22"/>
+      <c r="K80" s="22"/>
+      <c r="L80" s="22"/>
+      <c r="M80" s="22"/>
+    </row>
+    <row r="81" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B81" s="23" t="s">
+        <v>326</v>
+      </c>
+      <c r="C81" s="22" t="s">
+        <v>710</v>
+      </c>
+      <c r="D81" s="23"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="22"/>
+      <c r="H81" s="23"/>
+      <c r="I81" s="22"/>
+      <c r="J81" s="23"/>
+      <c r="K81" s="22"/>
+      <c r="L81" s="23"/>
+      <c r="M81" s="22"/>
+    </row>
+    <row r="82" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="22"/>
+      <c r="J82" s="22"/>
+      <c r="K82" s="22"/>
+      <c r="L82" s="22"/>
+      <c r="M82" s="22"/>
+    </row>
+    <row r="83" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
+      <c r="G83" s="22"/>
+      <c r="H83" s="22"/>
+      <c r="I83" s="22"/>
+      <c r="J83" s="22"/>
+      <c r="K83" s="22"/>
+      <c r="L83" s="22"/>
+      <c r="M83" s="22"/>
+    </row>
+    <row r="84" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B84" s="23" t="s">
+        <v>340</v>
+      </c>
+      <c r="C84" s="22" t="s">
+        <v>711</v>
+      </c>
+      <c r="D84" s="23"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="22"/>
+      <c r="H84" s="23"/>
+      <c r="I84" s="22"/>
+      <c r="J84" s="23"/>
+      <c r="K84" s="22"/>
+      <c r="L84" s="23"/>
+      <c r="M84" s="22"/>
+    </row>
+    <row r="85" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="22"/>
+      <c r="H85" s="22"/>
+      <c r="I85" s="22"/>
+      <c r="J85" s="22"/>
+      <c r="K85" s="22"/>
+      <c r="L85" s="22"/>
+      <c r="M85" s="22"/>
+    </row>
+    <row r="86" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
+      <c r="H86" s="22"/>
+      <c r="I86" s="22"/>
+      <c r="J86" s="22"/>
+      <c r="K86" s="22"/>
+      <c r="L86" s="22"/>
+      <c r="M86" s="22"/>
+    </row>
+    <row r="87" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B87" s="23" t="s">
+        <v>506</v>
+      </c>
+      <c r="C87" s="22" t="s">
+        <v>712</v>
+      </c>
+      <c r="D87" s="23"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="22"/>
+      <c r="H87" s="23"/>
+      <c r="I87" s="22"/>
+      <c r="J87" s="23"/>
+      <c r="K87" s="22"/>
+      <c r="L87" s="23"/>
+      <c r="M87" s="22"/>
+    </row>
+    <row r="88" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="22"/>
+      <c r="G88" s="22"/>
+      <c r="H88" s="22"/>
+      <c r="I88" s="22"/>
+      <c r="J88" s="22"/>
+      <c r="K88" s="22"/>
+      <c r="L88" s="22"/>
+      <c r="M88" s="22"/>
+    </row>
+    <row r="89" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B89" s="22"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="22"/>
+      <c r="F89" s="22"/>
+      <c r="G89" s="22"/>
+      <c r="H89" s="22"/>
+      <c r="I89" s="22"/>
+      <c r="J89" s="22"/>
+      <c r="K89" s="22"/>
+      <c r="L89" s="22"/>
+      <c r="M89" s="22"/>
+    </row>
+    <row r="90" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B90" s="23" t="s">
+        <v>717</v>
+      </c>
+      <c r="C90" s="22" t="s">
+        <v>713</v>
+      </c>
+      <c r="D90" s="23"/>
+      <c r="E90" s="22"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="22"/>
+      <c r="H90" s="23"/>
+      <c r="I90" s="22"/>
+      <c r="J90" s="23"/>
+      <c r="K90" s="22"/>
+      <c r="L90" s="23"/>
+      <c r="M90" s="22"/>
+    </row>
+    <row r="91" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="22"/>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="22"/>
+      <c r="J91" s="22"/>
+      <c r="K91" s="22"/>
+      <c r="L91" s="22"/>
+      <c r="M91" s="22"/>
+    </row>
+    <row r="92" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B92" s="22"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="22"/>
+      <c r="G92" s="22"/>
+      <c r="H92" s="22"/>
+      <c r="I92" s="22"/>
+      <c r="J92" s="22"/>
+      <c r="K92" s="22"/>
+      <c r="L92" s="22"/>
+      <c r="M92" s="22"/>
+    </row>
+    <row r="93" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B93" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="C93" s="22" t="s">
+        <v>715</v>
+      </c>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="22"/>
+      <c r="G93" s="22"/>
+      <c r="H93" s="22"/>
+      <c r="I93" s="22"/>
+      <c r="J93" s="22"/>
+      <c r="K93" s="22"/>
+      <c r="L93" s="22"/>
+      <c r="M93" s="22"/>
+    </row>
+    <row r="94" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B94" s="22"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="22"/>
+      <c r="F94" s="22"/>
+      <c r="G94" s="22"/>
+      <c r="H94" s="22"/>
+      <c r="I94" s="22"/>
+      <c r="J94" s="22"/>
+      <c r="K94" s="22"/>
+      <c r="L94" s="22"/>
+      <c r="M94" s="22"/>
+    </row>
+    <row r="95" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B95" s="22"/>
+      <c r="C95" s="22"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="22"/>
+      <c r="G95" s="22"/>
+      <c r="H95" s="22"/>
+      <c r="I95" s="22"/>
+      <c r="J95" s="22"/>
+      <c r="K95" s="22"/>
+      <c r="L95" s="22"/>
+      <c r="M95" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Pertanggal 3 April 2024 16:54 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/Accounting.TblChartOfAccount.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/Accounting.TblChartOfAccount.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9360" windowHeight="3330" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9360" windowHeight="3330" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Auto Link" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="QDC COA" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1701" uniqueCount="1066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="1086">
   <si>
     <t>RAW COA STRUCTURE</t>
   </si>
@@ -3223,12 +3224,312 @@
   <si>
     <t>3-9000</t>
   </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1-1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1-2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1-3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1-4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1-5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2-1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2-2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2-3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3-1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3-2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3-3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3-9</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>000</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3266,6 +3567,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial Narrow"/>
@@ -3310,7 +3618,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -3357,12 +3665,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -3406,12 +3727,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3424,6 +3739,42 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="4" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3967,53 +4318,53 @@
       </c>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="F3" s="22" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="F3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="6"/>
-      <c r="S3" s="21" t="s">
+      <c r="S3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="21"/>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="21"/>
-      <c r="X3" s="21"/>
-      <c r="Y3" s="21"/>
-      <c r="Z3" s="21"/>
-      <c r="AA3" s="21"/>
-      <c r="AB3" s="21"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="27"/>
       <c r="AC3" s="6"/>
-      <c r="AD3" s="21" t="s">
+      <c r="AD3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="AE3" s="21"/>
-      <c r="AF3" s="21"/>
-      <c r="AG3" s="21"/>
-      <c r="AH3" s="21"/>
-      <c r="AI3" s="21"/>
-      <c r="AJ3" s="21"/>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21"/>
-      <c r="AM3" s="21"/>
+      <c r="AE3" s="27"/>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="27"/>
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AM3" s="27"/>
       <c r="AN3" s="6"/>
       <c r="AO3" s="8" t="s">
         <v>673</v>
@@ -20930,7 +21281,7 @@
       <c r="O171" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="Q171" s="26" t="str">
+      <c r="Q171" s="24" t="str">
         <f t="shared" si="64"/>
         <v>Opening Balance - Material</v>
       </c>
@@ -21032,7 +21383,7 @@
       <c r="O172" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="Q172" s="26" t="str">
+      <c r="Q172" s="24" t="str">
         <f t="shared" si="64"/>
         <v>Opening Balance - Supplies</v>
       </c>
@@ -21134,7 +21485,7 @@
       <c r="O173" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="Q173" s="26" t="str">
+      <c r="Q173" s="24" t="str">
         <f t="shared" si="64"/>
         <v>Purchase - Material</v>
       </c>
@@ -21236,7 +21587,7 @@
       <c r="O174" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="Q174" s="26" t="str">
+      <c r="Q174" s="24" t="str">
         <f t="shared" si="64"/>
         <v>Purchase - Supplies</v>
       </c>
@@ -21338,7 +21689,7 @@
       <c r="O175" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="Q175" s="26" t="str">
+      <c r="Q175" s="24" t="str">
         <f t="shared" si="64"/>
         <v>Ending Balance - Material</v>
       </c>
@@ -21440,7 +21791,7 @@
       <c r="O176" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="Q176" s="26" t="str">
+      <c r="Q176" s="24" t="str">
         <f t="shared" si="64"/>
         <v>Ending Balance - Supplies</v>
       </c>
@@ -21542,7 +21893,7 @@
       <c r="O177" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="Q177" s="26" t="str">
+      <c r="Q177" s="24" t="str">
         <f t="shared" si="64"/>
         <v>Material Used</v>
       </c>
@@ -21644,7 +21995,7 @@
       <c r="O178" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="Q178" s="26" t="str">
+      <c r="Q178" s="24" t="str">
         <f t="shared" si="64"/>
         <v>Supplies Used</v>
       </c>
@@ -21746,7 +22097,7 @@
       <c r="O179" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="Q179" s="26" t="str">
+      <c r="Q179" s="24" t="str">
         <f t="shared" si="64"/>
         <v>Material Other</v>
       </c>
@@ -21848,7 +22199,7 @@
       <c r="O180" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="Q180" s="26" t="str">
+      <c r="Q180" s="24" t="str">
         <f t="shared" si="64"/>
         <v>IT Hardware Purchase</v>
       </c>
@@ -22052,7 +22403,7 @@
       <c r="O182" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="Q182" s="27" t="str">
+      <c r="Q182" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Salary Daily Worker</v>
       </c>
@@ -22154,7 +22505,7 @@
       <c r="O183" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="Q183" s="27" t="str">
+      <c r="Q183" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Salary Direct</v>
       </c>
@@ -22256,7 +22607,7 @@
       <c r="O184" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="Q184" s="27" t="str">
+      <c r="Q184" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Salary Indirect</v>
       </c>
@@ -22358,7 +22709,7 @@
       <c r="O185" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="Q185" s="27" t="str">
+      <c r="Q185" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Overtime Direct</v>
       </c>
@@ -22460,7 +22811,7 @@
       <c r="O186" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="Q186" s="27" t="str">
+      <c r="Q186" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Overtime Indirect</v>
       </c>
@@ -22562,7 +22913,7 @@
       <c r="O187" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="Q187" s="27" t="str">
+      <c r="Q187" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Jamsostek Direct</v>
       </c>
@@ -22664,7 +23015,7 @@
       <c r="O188" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="Q188" s="27" t="str">
+      <c r="Q188" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Jamsostek Indirect</v>
       </c>
@@ -22766,7 +23117,7 @@
       <c r="O189" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="Q189" s="27" t="str">
+      <c r="Q189" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Bonus,THR-Direct</v>
       </c>
@@ -22868,7 +23219,7 @@
       <c r="O190" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="Q190" s="27" t="str">
+      <c r="Q190" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Performance Bonus-Direct</v>
       </c>
@@ -22970,7 +23321,7 @@
       <c r="O191" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="Q191" s="27" t="str">
+      <c r="Q191" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Bonus,THR-Indirect</v>
       </c>
@@ -23072,7 +23423,7 @@
       <c r="O192" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="Q192" s="27" t="str">
+      <c r="Q192" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Performance Bonus-Indirect</v>
       </c>
@@ -23174,7 +23525,7 @@
       <c r="O193" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="Q193" s="27" t="str">
+      <c r="Q193" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Personal Income Tax-Direct</v>
       </c>
@@ -23276,7 +23627,7 @@
       <c r="O194" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="Q194" s="27" t="str">
+      <c r="Q194" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Personal Income Tax-Indirect</v>
       </c>
@@ -23378,7 +23729,7 @@
       <c r="O195" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="Q195" s="27" t="str">
+      <c r="Q195" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Uniform,Protect Clothe-Direct</v>
       </c>
@@ -23480,7 +23831,7 @@
       <c r="O196" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="Q196" s="27" t="str">
+      <c r="Q196" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Uniform,Protect Cloth-Indirect</v>
       </c>
@@ -23582,7 +23933,7 @@
       <c r="O197" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="Q197" s="27" t="str">
+      <c r="Q197" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Business Trip Allowance</v>
       </c>
@@ -23684,7 +24035,7 @@
       <c r="O198" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="Q198" s="27" t="str">
+      <c r="Q198" s="25" t="str">
         <f t="shared" si="64"/>
         <v>Meal</v>
       </c>
@@ -23786,7 +24137,7 @@
       <c r="O199" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="Q199" s="27" t="str">
+      <c r="Q199" s="25" t="str">
         <f t="shared" ref="Q199:Q262" si="86">D199</f>
         <v>Severance Pay - Project</v>
       </c>
@@ -23888,7 +24239,7 @@
       <c r="O200" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="Q200" s="27" t="str">
+      <c r="Q200" s="25" t="str">
         <f t="shared" si="86"/>
         <v>Sub Contractor</v>
       </c>
@@ -24092,7 +24443,7 @@
       <c r="O202" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="Q202" s="28" t="str">
+      <c r="Q202" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Consumables</v>
       </c>
@@ -24194,7 +24545,7 @@
       <c r="O203" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="Q203" s="28" t="str">
+      <c r="Q203" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Spare Parts</v>
       </c>
@@ -24296,7 +24647,7 @@
       <c r="O204" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="Q204" s="28" t="str">
+      <c r="Q204" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Tools</v>
       </c>
@@ -24398,7 +24749,7 @@
       <c r="O205" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="Q205" s="28" t="str">
+      <c r="Q205" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Utilities</v>
       </c>
@@ -24500,7 +24851,7 @@
       <c r="O206" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="Q206" s="28" t="str">
+      <c r="Q206" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Stationery &amp; Printing</v>
       </c>
@@ -24602,7 +24953,7 @@
       <c r="O207" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="Q207" s="28" t="str">
+      <c r="Q207" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Postage &amp; Courier Service</v>
       </c>
@@ -24704,7 +25055,7 @@
       <c r="O208" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="Q208" s="28" t="str">
+      <c r="Q208" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Telephone Expenses</v>
       </c>
@@ -24806,7 +25157,7 @@
       <c r="O209" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="Q209" s="28" t="str">
+      <c r="Q209" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Mobile Phone</v>
       </c>
@@ -24908,7 +25259,7 @@
       <c r="O210" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="Q210" s="28" t="str">
+      <c r="Q210" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Insurance Expenses</v>
       </c>
@@ -25010,7 +25361,7 @@
       <c r="O211" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="Q211" s="28" t="str">
+      <c r="Q211" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Property Rental/Lease</v>
       </c>
@@ -25112,7 +25463,7 @@
       <c r="O212" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="Q212" s="28" t="str">
+      <c r="Q212" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Hire of Other Plant &amp; Equipt</v>
       </c>
@@ -25214,7 +25565,7 @@
       <c r="O213" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="Q213" s="28" t="str">
+      <c r="Q213" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Property Repair &amp; Maintenance</v>
       </c>
@@ -25316,7 +25667,7 @@
       <c r="O214" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="Q214" s="28" t="str">
+      <c r="Q214" s="26" t="str">
         <f t="shared" si="86"/>
         <v>IT Expenses</v>
       </c>
@@ -25418,7 +25769,7 @@
       <c r="O215" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="Q215" s="28" t="str">
+      <c r="Q215" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Hire of Motor Vehicle</v>
       </c>
@@ -25520,7 +25871,7 @@
       <c r="O216" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="Q216" s="28" t="str">
+      <c r="Q216" s="26" t="str">
         <f t="shared" si="86"/>
         <v>MV-Fuel &amp; Oil</v>
       </c>
@@ -25622,7 +25973,7 @@
       <c r="O217" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="Q217" s="28" t="str">
+      <c r="Q217" s="26" t="str">
         <f t="shared" si="86"/>
         <v>MV-Repair &amp; Maintenance</v>
       </c>
@@ -25724,7 +26075,7 @@
       <c r="O218" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="Q218" s="28" t="str">
+      <c r="Q218" s="26" t="str">
         <f t="shared" si="86"/>
         <v>MV-Tyres, Tubes</v>
       </c>
@@ -25826,7 +26177,7 @@
       <c r="O219" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="Q219" s="28" t="str">
+      <c r="Q219" s="26" t="str">
         <f t="shared" si="86"/>
         <v>MV-Spare Parts</v>
       </c>
@@ -25928,7 +26279,7 @@
       <c r="O220" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="Q220" s="28" t="str">
+      <c r="Q220" s="26" t="str">
         <f t="shared" si="86"/>
         <v>MV-Accessories</v>
       </c>
@@ -26030,7 +26381,7 @@
       <c r="O221" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="Q221" s="28" t="str">
+      <c r="Q221" s="26" t="str">
         <f t="shared" si="86"/>
         <v>MV Other</v>
       </c>
@@ -26132,7 +26483,7 @@
       <c r="O222" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="Q222" s="28" t="str">
+      <c r="Q222" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Local Transport</v>
       </c>
@@ -26234,7 +26585,7 @@
       <c r="O223" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="Q223" s="28" t="str">
+      <c r="Q223" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Business Travelling</v>
       </c>
@@ -26336,7 +26687,7 @@
       <c r="O224" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="Q224" s="28" t="str">
+      <c r="Q224" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Travel &amp; Fares</v>
       </c>
@@ -26438,7 +26789,7 @@
       <c r="O225" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="Q225" s="28" t="str">
+      <c r="Q225" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Freight Expenses</v>
       </c>
@@ -26540,7 +26891,7 @@
       <c r="O226" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="Q226" s="28" t="str">
+      <c r="Q226" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Custom Clearance</v>
       </c>
@@ -26642,7 +26993,7 @@
       <c r="O227" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="Q227" s="28" t="str">
+      <c r="Q227" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Infrastructure</v>
       </c>
@@ -26744,7 +27095,7 @@
       <c r="O228" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="Q228" s="28" t="str">
+      <c r="Q228" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Tender Cost</v>
       </c>
@@ -26846,7 +27197,7 @@
       <c r="O229" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="Q229" s="28" t="str">
+      <c r="Q229" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Sitac Expenses</v>
       </c>
@@ -26948,7 +27299,7 @@
       <c r="O230" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="Q230" s="28" t="str">
+      <c r="Q230" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Loss, Damage &amp; Pinalty</v>
       </c>
@@ -27050,7 +27401,7 @@
       <c r="O231" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="Q231" s="28" t="str">
+      <c r="Q231" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Supervision Expenses</v>
       </c>
@@ -27152,7 +27503,7 @@
       <c r="O232" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="Q232" s="28" t="str">
+      <c r="Q232" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Power Supply</v>
       </c>
@@ -27254,7 +27605,7 @@
       <c r="O233" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="Q233" s="28" t="str">
+      <c r="Q233" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Civil  Work</v>
       </c>
@@ -27356,7 +27707,7 @@
       <c r="O234" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="Q234" s="28" t="str">
+      <c r="Q234" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Moblilization &amp; demobilization</v>
       </c>
@@ -27458,7 +27809,7 @@
       <c r="O235" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="Q235" s="28" t="str">
+      <c r="Q235" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Entertainment-Deductable</v>
       </c>
@@ -27560,7 +27911,7 @@
       <c r="O236" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="Q236" s="28" t="str">
+      <c r="Q236" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Entertainment-Undeductable</v>
       </c>
@@ -27662,7 +28013,7 @@
       <c r="O237" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="Q237" s="28" t="str">
+      <c r="Q237" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Non Meal Entertaint-Ded.</v>
       </c>
@@ -27764,7 +28115,7 @@
       <c r="O238" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="Q238" s="28" t="str">
+      <c r="Q238" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Non Meal Entertaint-Unded.</v>
       </c>
@@ -27866,7 +28217,7 @@
       <c r="O239" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="Q239" s="28" t="str">
+      <c r="Q239" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Donation</v>
       </c>
@@ -27968,7 +28319,7 @@
       <c r="O240" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="Q240" s="28" t="str">
+      <c r="Q240" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Depre - Building Improvement</v>
       </c>
@@ -28070,7 +28421,7 @@
       <c r="O241" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="Q241" s="28" t="str">
+      <c r="Q241" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Depre - IT Equipment</v>
       </c>
@@ -28172,7 +28523,7 @@
       <c r="O242" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="Q242" s="28" t="str">
+      <c r="Q242" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Depre - Office Machine &amp; Equip</v>
       </c>
@@ -28274,7 +28625,7 @@
       <c r="O243" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="Q243" s="28" t="str">
+      <c r="Q243" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Depre - Sundry Plant &amp; Equipt</v>
       </c>
@@ -28376,7 +28727,7 @@
       <c r="O244" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="Q244" s="28" t="str">
+      <c r="Q244" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Depre - Test Equipment</v>
       </c>
@@ -28478,7 +28829,7 @@
       <c r="O245" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="Q245" s="28" t="str">
+      <c r="Q245" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Depre - Motor Vehicle</v>
       </c>
@@ -28580,7 +28931,7 @@
       <c r="O246" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="Q246" s="28" t="str">
+      <c r="Q246" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Depre - Tools</v>
       </c>
@@ -28682,7 +29033,7 @@
       <c r="O247" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="Q247" s="28" t="str">
+      <c r="Q247" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Depre - Furniture Fitting</v>
       </c>
@@ -28784,7 +29135,7 @@
       <c r="O248" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="Q248" s="28" t="str">
+      <c r="Q248" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Depre - Mobile Phone</v>
       </c>
@@ -28886,7 +29237,7 @@
       <c r="O249" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="Q249" s="28" t="str">
+      <c r="Q249" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Customer Claims</v>
       </c>
@@ -28988,7 +29339,7 @@
       <c r="O250" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="Q250" s="28" t="str">
+      <c r="Q250" s="26" t="str">
         <f t="shared" si="86"/>
         <v>Other Overhead</v>
       </c>
@@ -38615,9 +38966,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M296"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I273" sqref="I273"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D102" sqref="D102:E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -38639,30 +38990,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23" t="s">
+      <c r="E2" s="29"/>
+      <c r="F2" s="29" t="s">
         <v>742</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29" t="s">
         <v>743</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23" t="s">
+      <c r="I2" s="29"/>
+      <c r="J2" s="29" t="s">
         <v>744</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23" t="s">
+      <c r="K2" s="29"/>
+      <c r="L2" s="29" t="s">
         <v>745</v>
       </c>
-      <c r="M2" s="23"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
@@ -40315,7 +40666,7 @@
       <c r="H86" s="20" t="s">
         <v>868</v>
       </c>
-      <c r="I86" s="25" t="s">
+      <c r="I86" s="23" t="s">
         <v>273</v>
       </c>
       <c r="J86" s="19"/>
@@ -40352,7 +40703,7 @@
         <v>265</v>
       </c>
       <c r="H88" s="20"/>
-      <c r="I88" s="25"/>
+      <c r="I88" s="23"/>
       <c r="J88" s="19"/>
       <c r="K88" s="19"/>
       <c r="L88" s="19"/>
@@ -40504,7 +40855,7 @@
     <row r="97" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B97" s="19"/>
       <c r="C97" s="19"/>
-      <c r="D97" s="24" t="s">
+      <c r="D97" s="22" t="s">
         <v>858</v>
       </c>
       <c r="E97" s="19" t="s">
@@ -40512,7 +40863,7 @@
       </c>
       <c r="F97" s="19"/>
       <c r="G97" s="19"/>
-      <c r="H97" s="24" t="s">
+      <c r="H97" s="22" t="s">
         <v>880</v>
       </c>
       <c r="I97" s="15" t="s">
@@ -40526,11 +40877,11 @@
     <row r="98" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B98" s="19"/>
       <c r="C98" s="19"/>
-      <c r="D98" s="24"/>
+      <c r="D98" s="22"/>
       <c r="E98" s="19"/>
       <c r="F98" s="19"/>
       <c r="G98" s="19"/>
-      <c r="H98" s="24" t="s">
+      <c r="H98" s="22" t="s">
         <v>894</v>
       </c>
       <c r="I98" s="19" t="s">
@@ -40544,11 +40895,11 @@
     <row r="99" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B99" s="19"/>
       <c r="C99" s="19"/>
-      <c r="D99" s="24"/>
+      <c r="D99" s="22"/>
       <c r="E99" s="19"/>
       <c r="F99" s="19"/>
       <c r="G99" s="19"/>
-      <c r="H99" s="24" t="s">
+      <c r="H99" s="22" t="s">
         <v>896</v>
       </c>
       <c r="I99" s="19" t="s">
@@ -40562,11 +40913,11 @@
     <row r="100" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B100" s="19"/>
       <c r="C100" s="19"/>
-      <c r="D100" s="24"/>
+      <c r="D100" s="22"/>
       <c r="E100" s="19"/>
       <c r="F100" s="19"/>
       <c r="G100" s="19"/>
-      <c r="H100" s="24" t="s">
+      <c r="H100" s="22" t="s">
         <v>895</v>
       </c>
       <c r="I100" s="19" t="s">
@@ -40580,11 +40931,11 @@
     <row r="101" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B101" s="19"/>
       <c r="C101" s="19"/>
-      <c r="D101" s="24"/>
+      <c r="D101" s="22"/>
       <c r="E101" s="19"/>
       <c r="F101" s="19"/>
       <c r="G101" s="19"/>
-      <c r="H101" s="24"/>
+      <c r="H101" s="22"/>
       <c r="I101" s="19"/>
       <c r="J101" s="19"/>
       <c r="K101" s="19"/>
@@ -44056,4 +44407,586 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="30"/>
+    <col min="2" max="2" width="5.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="29"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>746</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="32" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>707</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="31"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="33"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="33" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="33"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="31"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="33"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="34" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="33"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="33"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="34" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="33"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="33"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="34" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="33"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="19"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="33"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="34" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="33"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="19"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="38"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="34" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>708</v>
+      </c>
+      <c r="D16" s="33"/>
+      <c r="E16" s="31"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="33"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="34" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="33"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="33"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="34" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="33"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="31"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="33"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="37" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="33"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="31"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="39"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="34" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>709</v>
+      </c>
+      <c r="D24" s="33"/>
+      <c r="E24" s="31"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="35"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="34" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="33"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="31"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="35"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="34" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="33"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="31"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="35"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="34" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="35"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="19"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="35"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="34" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="35"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="19"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="40"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="41"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="34" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>710</v>
+      </c>
+      <c r="D34" s="34"/>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="34"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="19"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="34"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="19"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="34"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="19"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="34"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="35"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="19"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="35"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="19"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="34" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>711</v>
+      </c>
+      <c r="D41" s="34"/>
+      <c r="E41" s="19"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="34"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="19"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="34"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="19"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="34"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="19"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="34"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="19"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="35"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="19"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="35"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="19"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="34"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="19"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="34"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="19"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="34"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="19"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="34" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>712</v>
+      </c>
+      <c r="D51" s="34"/>
+      <c r="E51" s="19"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="34"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="19"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="34"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="19"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="34"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="19"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="34"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="19"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="34"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="19"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="34"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="19"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="34"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="19"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="34"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="19"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="34" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>713</v>
+      </c>
+      <c r="D60" s="34"/>
+      <c r="E60" s="19"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="34"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="19"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="34"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="19"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B63" s="34"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="19"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B64" s="34"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="19"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B65" s="34"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="19"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B66" s="34"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="19"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B67" s="34"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="19"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B68" s="34"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="19"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="35" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>715</v>
+      </c>
+      <c r="D69" s="34"/>
+      <c r="E69" s="19"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B70" s="35"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="19"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B71" s="35"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="19"/>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B72" s="35"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="19"/>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B73" s="35"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="19"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B74" s="35"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="19"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B75" s="35"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="19"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B76" s="35"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="19"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B77" s="35"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="19"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B78" s="35"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>